<commit_message>
update doc, set expired date on01/07/2024
</commit_message>
<xml_diff>
--- a/data_test/240222_ Power-effect_285nm samples.xlsx
+++ b/data_test/240222_ Power-effect_285nm samples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\205-Caracterisation_Metrologie\205.00-Stages_Theses_Postdoc\2023-JAMIL Rayan\Technique\Données\Raman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VL251876\Documents\Python\SPECTROview\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -260,9 +260,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Power(ND%)</t>
-  </si>
-  <si>
     <t>After_high_power</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>1ML-285nm_532nm_high_p01_100x_10sx5</t>
+  </si>
+  <si>
+    <t>Laser Power</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,7 @@
     <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -754,10 +754,10 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>57</v>
@@ -811,12 +811,12 @@
         <v>73</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -900,7 +900,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3">
         <v>1883.14</v>
@@ -972,7 +972,7 @@
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4">
         <v>2072.59</v>
@@ -1620,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13">
         <v>4231.72</v>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14">
         <v>6710.72</v>
@@ -1764,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>6357.37</v>
@@ -2124,7 +2124,7 @@
         <v>0.5</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20">
         <v>5155.2</v>
@@ -2196,7 +2196,7 @@
         <v>0.5</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21">
         <v>3427.84</v>
@@ -2268,7 +2268,7 @@
         <v>0.5</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22">
         <v>912.58</v>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F30">
         <v>13099.6</v>
@@ -2916,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F31">
         <v>9801.9699999999993</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
         <v>74</v>
@@ -2988,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F32">
         <v>14033.3</v>
@@ -3420,7 +3420,7 @@
         <v>0.1</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F38">
         <v>1773.74</v>
@@ -3492,7 +3492,7 @@
         <v>0.1</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F39">
         <v>1353.77</v>
@@ -3564,7 +3564,7 @@
         <v>0.1</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40">
         <v>914.78200000000004</v>
@@ -4428,7 +4428,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F52">
         <v>9913.6</v>
@@ -4500,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F53">
         <v>7568.11</v>

</xml_diff>